<commit_message>
funcoinadno la factura la recueracion de excel
</commit_message>
<xml_diff>
--- a/back/public/a.xlsx
+++ b/back/public/a.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adimer\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyectos\nautica\back\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4C7EE4-1CE5-4D4F-87DA-0605537CCB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A4EE07E-C9EE-4C88-8F4B-EAD0FD08D917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{598F938E-DE4E-4079-B807-48A48DF4BEFC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$12:$M$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -84,6 +79,12 @@
     <t>Resumen</t>
   </si>
   <si>
+    <t>Unidad</t>
+  </si>
+  <si>
+    <t>Precio</t>
+  </si>
+  <si>
     <t>Venta</t>
   </si>
   <si>
@@ -91,12 +92,6 @@
   </si>
   <si>
     <t>Totales</t>
-  </si>
-  <si>
-    <t>Unidad</t>
-  </si>
-  <si>
-    <t>Precio</t>
   </si>
 </sst>
 </file>
@@ -104,27 +99,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -139,8 +126,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+        <fgColor rgb="FF9DC3E6"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -153,27 +140,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="60% - Énfasis5" xfId="1" builtinId="48"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -190,60 +175,43 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
+      <xdr:colOff>409575</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>198120</xdr:colOff>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>46044</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCF31970-5398-8451-7BCD-5D231C465EB4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="9898380" y="99060"/>
-          <a:ext cx="1371600" cy="678504"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1371600" cy="676275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -252,7 +220,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -294,7 +262,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -346,7 +314,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -407,165 +375,189 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770755DC-C827-423E-9EFE-A4D1CCCC3548}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.77734375" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -626,23 +618,23 @@
         <v>17</v>
       </c>
       <c r="I12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="M12" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A12:M12" xr:uid="{770755DC-C827-423E-9EFE-A4D1CCCC3548}"/>
+  <autoFilter ref="A12:M12" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
funicoandano la creacion del excel
</commit_message>
<xml_diff>
--- a/back/public/a.xlsx
+++ b/back/public/a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyectos\nautica\back\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A4EE07E-C9EE-4C88-8F4B-EAD0FD08D917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2B34A37-DE43-4E2F-BA2D-61BF250A8873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -543,15 +543,15 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="20.77734375" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
@@ -592,6 +592,16 @@
         <v>9</v>
       </c>
     </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K11">
+        <f>SUM(K13:K1020)</f>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f>SUM(L13:L1020)</f>
+        <v>0</v>
+      </c>
+    </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>10</v>

</xml_diff>